<commit_message>
Tijdreeks voorbeeld omgezet in een taak
</commit_message>
<xml_diff>
--- a/resources/Excel_Screendumps_NL.xlsx
+++ b/resources/Excel_Screendumps_NL.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\office\leerexcel\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A4E17D-1456-49E1-9250-0AEBEB4040C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81486225-F446-4F8B-B839-4F40AD7DF606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="901" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="901" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Componenten" sheetId="68" r:id="rId1"/>
-    <sheet name="ausbeer" sheetId="69" r:id="rId2"/>
+    <sheet name="ausbeer56-73" sheetId="69" r:id="rId2"/>
     <sheet name="ausbeer-1" sheetId="71" r:id="rId3"/>
     <sheet name="ausbeer-2" sheetId="72" r:id="rId4"/>
     <sheet name="ausbeer-3" sheetId="73" r:id="rId5"/>
@@ -191,7 +191,7 @@
     <pivotCache cacheId="1" r:id="rId70"/>
     <pivotCache cacheId="2" r:id="rId71"/>
     <pivotCache cacheId="3" r:id="rId72"/>
-    <pivotCache cacheId="9" r:id="rId73"/>
+    <pivotCache cacheId="4" r:id="rId73"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2745,6 +2745,11 @@
     <xf numFmtId="178" fontId="11" fillId="0" borderId="0" xfId="35" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="35" applyFont="1"/>
     <xf numFmtId="172" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="35" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="33" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2785,11 +2790,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="0" xfId="35" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="40">
     <cellStyle name="Categorietitel" xfId="28" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2834,9 +2834,6 @@
     <cellStyle name="Valuta 8" xfId="26" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2891,6 +2888,9 @@
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -6229,6 +6229,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="19050" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -7510,6 +7513,74 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:ln w="19050" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -7544,11 +7615,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:srgbClr val="C00000"/>
+                  <a:schemeClr val="accent1"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10871,6 +10942,9 @@
       <c:pivotFmt>
         <c:idx val="19"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="19050" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -10939,6 +11013,9 @@
       <c:pivotFmt>
         <c:idx val="20"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11007,6 +11084,9 @@
       <c:pivotFmt>
         <c:idx val="21"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11075,6 +11155,9 @@
       <c:pivotFmt>
         <c:idx val="22"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11143,6 +11226,9 @@
       <c:pivotFmt>
         <c:idx val="23"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11211,6 +11297,9 @@
       <c:pivotFmt>
         <c:idx val="24"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11279,6 +11368,9 @@
       <c:pivotFmt>
         <c:idx val="25"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11347,6 +11439,9 @@
       <c:pivotFmt>
         <c:idx val="26"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11415,6 +11510,9 @@
       <c:pivotFmt>
         <c:idx val="27"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11483,6 +11581,9 @@
       <c:pivotFmt>
         <c:idx val="28"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11551,6 +11652,9 @@
       <c:pivotFmt>
         <c:idx val="29"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11619,6 +11723,9 @@
       <c:pivotFmt>
         <c:idx val="30"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11687,6 +11794,9 @@
       <c:pivotFmt>
         <c:idx val="31"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11755,6 +11865,9 @@
       <c:pivotFmt>
         <c:idx val="32"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11823,6 +11936,9 @@
       <c:pivotFmt>
         <c:idx val="33"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11891,6 +12007,9 @@
       <c:pivotFmt>
         <c:idx val="34"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -11959,6 +12078,9 @@
       <c:pivotFmt>
         <c:idx val="35"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -12027,6 +12149,9 @@
       <c:pivotFmt>
         <c:idx val="36"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -12095,6 +12220,9 @@
       <c:pivotFmt>
         <c:idx val="37"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -12317,6 +12445,74 @@
             <a:ln w="9525">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="41"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -29754,8 +29950,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>532725</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -29796,7 +29992,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>75524</xdr:colOff>
+      <xdr:colOff>161924</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
@@ -29839,7 +30035,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>466049</xdr:colOff>
+      <xdr:colOff>552449</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
@@ -36031,7 +36227,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95AE08B7-D928-4FBF-B7C0-E134C75D42B9}" name="ausbeer1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95AE08B7-D928-4FBF-B7C0-E134C75D42B9}" name="ausbeer1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A1:B92" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField numFmtId="14" showAll="0">
@@ -36400,7 +36596,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9EDFBDBB-B433-4E16-A04D-3195E601D6D4}" name="ausbeer2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9EDFBDBB-B433-4E16-A04D-3195E601D6D4}" name="ausbeer2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A1:T7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField numFmtId="14" showAll="0">
@@ -36545,7 +36741,7 @@
   <dataFields count="1">
     <dataField name="Bierproductie" fld="1" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <chartFormats count="19">
+  <chartFormats count="20">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -36768,6 +36964,18 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="1" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -36782,7 +36990,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E449110E-89DC-4DF2-B822-02FC3842901E}" name="ausbeer3" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E449110E-89DC-4DF2-B822-02FC3842901E}" name="ausbeer3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Waarden" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A1:F21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField numFmtId="14" showAll="0">
@@ -36927,7 +37135,7 @@
   <dataFields count="1">
     <dataField name="Bierproductie" fld="1" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
-  <chartFormats count="41">
+  <chartFormats count="50">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -37411,6 +37619,114 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="2" format="41" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="42" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="43" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="44" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="5" format="45" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="46" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="47" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="48" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="6" format="49" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -37638,29 +37954,29 @@
     <dataField name="Som van Omzet" fld="2" baseField="0" baseItem="0" numFmtId="5"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="7">
+    <format dxfId="6">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="5">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="5">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="4">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="2">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="2">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -37766,7 +38082,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{407A0BE2-4F90-4F81-AF2A-B154C2D85555}" name="ausbeer56_73" displayName="ausbeer56_73" ref="A1:B73" totalsRowShown="0">
   <autoFilter ref="A1:B73" xr:uid="{D3D07369-F3F9-4FCF-889E-7A3D40310FAD}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0D8F5C0E-9192-4F34-B66A-412DA346C977}" name="Datum" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0D8F5C0E-9192-4F34-B66A-412DA346C977}" name="Datum" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{DCD143B9-BBC2-44AA-86B1-AA5A8830F651}" name="Volume"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -39112,11 +39428,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.15">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="228" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="179" t="s">
@@ -39575,7 +39891,7 @@
   <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39594,7 +39910,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="239">
+      <c r="A2" s="225">
         <v>20455</v>
       </c>
       <c r="B2" s="201">
@@ -39602,7 +39918,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="239">
+      <c r="A3" s="225">
         <v>20546</v>
       </c>
       <c r="B3" s="201">
@@ -39610,7 +39926,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="239">
+      <c r="A4" s="225">
         <v>20637</v>
       </c>
       <c r="B4" s="201">
@@ -39618,7 +39934,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="239">
+      <c r="A5" s="225">
         <v>20729</v>
       </c>
       <c r="B5" s="201">
@@ -39626,7 +39942,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="239">
+      <c r="A6" s="225">
         <v>20821</v>
       </c>
       <c r="B6" s="201">
@@ -39634,7 +39950,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="239">
+      <c r="A7" s="225">
         <v>20911</v>
       </c>
       <c r="B7" s="201">
@@ -39642,7 +39958,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="239">
+      <c r="A8" s="225">
         <v>21002</v>
       </c>
       <c r="B8" s="201">
@@ -39650,7 +39966,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="239">
+      <c r="A9" s="225">
         <v>21094</v>
       </c>
       <c r="B9" s="201">
@@ -39658,7 +39974,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="239">
+      <c r="A10" s="225">
         <v>21186</v>
       </c>
       <c r="B10" s="201">
@@ -39666,7 +39982,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="239">
+      <c r="A11" s="225">
         <v>21276</v>
       </c>
       <c r="B11" s="201">
@@ -39674,7 +39990,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="239">
+      <c r="A12" s="225">
         <v>21367</v>
       </c>
       <c r="B12" s="201">
@@ -39682,7 +39998,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="239">
+      <c r="A13" s="225">
         <v>21459</v>
       </c>
       <c r="B13" s="201">
@@ -39690,7 +40006,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="239">
+      <c r="A14" s="225">
         <v>21551</v>
       </c>
       <c r="B14" s="201">
@@ -39698,7 +40014,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="239">
+      <c r="A15" s="225">
         <v>21641</v>
       </c>
       <c r="B15" s="201">
@@ -39706,7 +40022,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="239">
+      <c r="A16" s="225">
         <v>21732</v>
       </c>
       <c r="B16" s="201">
@@ -39714,7 +40030,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="239">
+      <c r="A17" s="225">
         <v>21824</v>
       </c>
       <c r="B17" s="201">
@@ -39722,7 +40038,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="239">
+      <c r="A18" s="225">
         <v>21916</v>
       </c>
       <c r="B18" s="201">
@@ -39730,7 +40046,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="239">
+      <c r="A19" s="225">
         <v>22007</v>
       </c>
       <c r="B19" s="201">
@@ -39738,7 +40054,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="239">
+      <c r="A20" s="225">
         <v>22098</v>
       </c>
       <c r="B20" s="201">
@@ -39746,7 +40062,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="239">
+      <c r="A21" s="225">
         <v>22190</v>
       </c>
       <c r="B21" s="201">
@@ -39754,7 +40070,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="239">
+      <c r="A22" s="225">
         <v>22282</v>
       </c>
       <c r="B22" s="201">
@@ -39762,7 +40078,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="239">
+      <c r="A23" s="225">
         <v>22372</v>
       </c>
       <c r="B23" s="201">
@@ -39770,7 +40086,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="239">
+      <c r="A24" s="225">
         <v>22463</v>
       </c>
       <c r="B24" s="201">
@@ -39778,7 +40094,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="239">
+      <c r="A25" s="225">
         <v>22555</v>
       </c>
       <c r="B25" s="201">
@@ -39786,7 +40102,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="239">
+      <c r="A26" s="225">
         <v>22647</v>
       </c>
       <c r="B26" s="201">
@@ -39794,7 +40110,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="239">
+      <c r="A27" s="225">
         <v>22737</v>
       </c>
       <c r="B27" s="201">
@@ -39802,7 +40118,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="239">
+      <c r="A28" s="225">
         <v>22828</v>
       </c>
       <c r="B28" s="201">
@@ -39810,7 +40126,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="239">
+      <c r="A29" s="225">
         <v>22920</v>
       </c>
       <c r="B29" s="201">
@@ -39818,7 +40134,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="239">
+      <c r="A30" s="225">
         <v>23012</v>
       </c>
       <c r="B30" s="201">
@@ -39826,7 +40142,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="239">
+      <c r="A31" s="225">
         <v>23102</v>
       </c>
       <c r="B31" s="201">
@@ -39834,7 +40150,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="239">
+      <c r="A32" s="225">
         <v>23193</v>
       </c>
       <c r="B32" s="201">
@@ -39842,7 +40158,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="239">
+      <c r="A33" s="225">
         <v>23285</v>
       </c>
       <c r="B33" s="201">
@@ -39850,7 +40166,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="239">
+      <c r="A34" s="225">
         <v>23377</v>
       </c>
       <c r="B34" s="201">
@@ -39858,7 +40174,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="239">
+      <c r="A35" s="225">
         <v>23468</v>
       </c>
       <c r="B35" s="201">
@@ -39866,7 +40182,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="239">
+      <c r="A36" s="225">
         <v>23559</v>
       </c>
       <c r="B36" s="201">
@@ -39874,7 +40190,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="239">
+      <c r="A37" s="225">
         <v>23651</v>
       </c>
       <c r="B37" s="201">
@@ -39882,7 +40198,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="239">
+      <c r="A38" s="225">
         <v>23743</v>
       </c>
       <c r="B38" s="201">
@@ -39890,7 +40206,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="239">
+      <c r="A39" s="225">
         <v>23833</v>
       </c>
       <c r="B39" s="201">
@@ -39898,7 +40214,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="239">
+      <c r="A40" s="225">
         <v>23924</v>
       </c>
       <c r="B40" s="201">
@@ -39906,7 +40222,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="239">
+      <c r="A41" s="225">
         <v>24016</v>
       </c>
       <c r="B41" s="201">
@@ -39914,7 +40230,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="239">
+      <c r="A42" s="225">
         <v>24108</v>
       </c>
       <c r="B42" s="201">
@@ -39922,7 +40238,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="239">
+      <c r="A43" s="225">
         <v>24198</v>
       </c>
       <c r="B43" s="201">
@@ -39930,7 +40246,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="239">
+      <c r="A44" s="225">
         <v>24289</v>
       </c>
       <c r="B44" s="201">
@@ -39938,7 +40254,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="239">
+      <c r="A45" s="225">
         <v>24381</v>
       </c>
       <c r="B45" s="201">
@@ -39946,7 +40262,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="239">
+      <c r="A46" s="225">
         <v>24473</v>
       </c>
       <c r="B46" s="201">
@@ -39954,7 +40270,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="239">
+      <c r="A47" s="225">
         <v>24563</v>
       </c>
       <c r="B47" s="201">
@@ -39962,7 +40278,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="239">
+      <c r="A48" s="225">
         <v>24654</v>
       </c>
       <c r="B48" s="201">
@@ -39970,7 +40286,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="239">
+      <c r="A49" s="225">
         <v>24746</v>
       </c>
       <c r="B49" s="201">
@@ -39978,7 +40294,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="239">
+      <c r="A50" s="225">
         <v>24838</v>
       </c>
       <c r="B50" s="201">
@@ -39986,7 +40302,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="239">
+      <c r="A51" s="225">
         <v>24929</v>
       </c>
       <c r="B51" s="201">
@@ -39994,7 +40310,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="239">
+      <c r="A52" s="225">
         <v>25020</v>
       </c>
       <c r="B52" s="201">
@@ -40002,7 +40318,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="239">
+      <c r="A53" s="225">
         <v>25112</v>
       </c>
       <c r="B53" s="201">
@@ -40010,7 +40326,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="239">
+      <c r="A54" s="225">
         <v>25204</v>
       </c>
       <c r="B54" s="201">
@@ -40018,7 +40334,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="239">
+      <c r="A55" s="225">
         <v>25294</v>
       </c>
       <c r="B55" s="201">
@@ -40026,7 +40342,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="239">
+      <c r="A56" s="225">
         <v>25385</v>
       </c>
       <c r="B56" s="201">
@@ -40034,7 +40350,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="239">
+      <c r="A57" s="225">
         <v>25477</v>
       </c>
       <c r="B57" s="201">
@@ -40042,7 +40358,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="239">
+      <c r="A58" s="225">
         <v>25569</v>
       </c>
       <c r="B58" s="201">
@@ -40050,7 +40366,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="239">
+      <c r="A59" s="225">
         <v>25659</v>
       </c>
       <c r="B59" s="201">
@@ -40058,7 +40374,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="239">
+      <c r="A60" s="225">
         <v>25750</v>
       </c>
       <c r="B60" s="201">
@@ -40066,7 +40382,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="239">
+      <c r="A61" s="225">
         <v>25842</v>
       </c>
       <c r="B61" s="201">
@@ -40074,7 +40390,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="239">
+      <c r="A62" s="225">
         <v>25934</v>
       </c>
       <c r="B62" s="201">
@@ -40082,7 +40398,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="239">
+      <c r="A63" s="225">
         <v>26024</v>
       </c>
       <c r="B63" s="201">
@@ -40090,7 +40406,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="239">
+      <c r="A64" s="225">
         <v>26115</v>
       </c>
       <c r="B64" s="201">
@@ -40098,7 +40414,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="239">
+      <c r="A65" s="225">
         <v>26207</v>
       </c>
       <c r="B65" s="201">
@@ -40106,7 +40422,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="239">
+      <c r="A66" s="225">
         <v>26299</v>
       </c>
       <c r="B66" s="201">
@@ -40114,7 +40430,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="239">
+      <c r="A67" s="225">
         <v>26390</v>
       </c>
       <c r="B67" s="201">
@@ -40122,7 +40438,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="239">
+      <c r="A68" s="225">
         <v>26481</v>
       </c>
       <c r="B68" s="201">
@@ -40130,7 +40446,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="239">
+      <c r="A69" s="225">
         <v>26573</v>
       </c>
       <c r="B69" s="201">
@@ -40138,7 +40454,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="239">
+      <c r="A70" s="225">
         <v>26665</v>
       </c>
       <c r="B70" s="201">
@@ -40146,7 +40462,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="239">
+      <c r="A71" s="225">
         <v>26755</v>
       </c>
       <c r="B71" s="201">
@@ -40154,7 +40470,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="239">
+      <c r="A72" s="225">
         <v>26846</v>
       </c>
       <c r="B72" s="201">
@@ -40162,7 +40478,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="239">
+      <c r="A73" s="225">
         <v>26938</v>
       </c>
       <c r="B73" s="201">
@@ -51918,7 +52234,7 @@
   <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51939,39 +52255,39 @@
       <c r="A2" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="B2" s="241">
+      <c r="B2" s="227">
         <v>1032</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="240" t="s">
+      <c r="A3" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="241">
+      <c r="B3" s="227">
         <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="240" t="s">
+      <c r="A4" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="241">
+      <c r="B4" s="227">
         <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="240" t="s">
+      <c r="A5" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="241">
+      <c r="B5" s="227">
         <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="240" t="s">
+      <c r="A6" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="241">
+      <c r="B6" s="227">
         <v>308</v>
       </c>
     </row>
@@ -51979,39 +52295,39 @@
       <c r="A7" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B7" s="241">
+      <c r="B7" s="227">
         <v>1046</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="240" t="s">
+      <c r="A8" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="241">
+      <c r="B8" s="227">
         <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="240" t="s">
+      <c r="A9" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="241">
+      <c r="B9" s="227">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="240" t="s">
+      <c r="A10" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="241">
+      <c r="B10" s="227">
         <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="240" t="s">
+      <c r="A11" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="241">
+      <c r="B11" s="227">
         <v>320</v>
       </c>
     </row>
@@ -52019,39 +52335,39 @@
       <c r="A12" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="B12" s="241">
+      <c r="B12" s="227">
         <v>1055</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="240" t="s">
+      <c r="A13" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="241">
+      <c r="B13" s="227">
         <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="240" t="s">
+      <c r="A14" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="241">
+      <c r="B14" s="227">
         <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="240" t="s">
+      <c r="A15" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="241">
+      <c r="B15" s="227">
         <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="240" t="s">
+      <c r="A16" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="241">
+      <c r="B16" s="227">
         <v>313</v>
       </c>
     </row>
@@ -52059,39 +52375,39 @@
       <c r="A17" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="B17" s="241">
+      <c r="B17" s="227">
         <v>1052</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="240" t="s">
+      <c r="A18" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B18" s="241">
+      <c r="B18" s="227">
         <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="240" t="s">
+      <c r="A19" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="241">
+      <c r="B19" s="227">
         <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="240" t="s">
+      <c r="A20" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B20" s="241">
+      <c r="B20" s="227">
         <v>250</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="240" t="s">
+      <c r="A21" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="241">
+      <c r="B21" s="227">
         <v>314</v>
       </c>
     </row>
@@ -52099,39 +52415,39 @@
       <c r="A22" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="B22" s="241">
+      <c r="B22" s="227">
         <v>1084</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="240" t="s">
+      <c r="A23" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="241">
+      <c r="B23" s="227">
         <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="240" t="s">
+      <c r="A24" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="241">
+      <c r="B24" s="227">
         <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="240" t="s">
+      <c r="A25" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="241">
+      <c r="B25" s="227">
         <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="240" t="s">
+      <c r="A26" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="241">
+      <c r="B26" s="227">
         <v>311</v>
       </c>
     </row>
@@ -52139,39 +52455,39 @@
       <c r="A27" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B27" s="241">
+      <c r="B27" s="227">
         <v>1124</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="240" t="s">
+      <c r="A28" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="241">
+      <c r="B28" s="227">
         <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="240" t="s">
+      <c r="A29" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="241">
+      <c r="B29" s="227">
         <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="240" t="s">
+      <c r="A30" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B30" s="241">
+      <c r="B30" s="227">
         <v>257</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="240" t="s">
+      <c r="A31" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B31" s="241">
+      <c r="B31" s="227">
         <v>339</v>
       </c>
     </row>
@@ -52179,39 +52495,39 @@
       <c r="A32" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="B32" s="241">
+      <c r="B32" s="227">
         <v>1145</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="240" t="s">
+      <c r="A33" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="241">
+      <c r="B33" s="227">
         <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="240" t="s">
+      <c r="A34" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="241">
+      <c r="B34" s="227">
         <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="240" t="s">
+      <c r="A35" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="241">
+      <c r="B35" s="227">
         <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="240" t="s">
+      <c r="A36" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="241">
+      <c r="B36" s="227">
         <v>346</v>
       </c>
     </row>
@@ -52219,39 +52535,39 @@
       <c r="A37" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="B37" s="241">
+      <c r="B37" s="227">
         <v>1190</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="240" t="s">
+      <c r="A38" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="241">
+      <c r="B38" s="227">
         <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="240" t="s">
+      <c r="A39" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="241">
+      <c r="B39" s="227">
         <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="240" t="s">
+      <c r="A40" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="241">
+      <c r="B40" s="227">
         <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="240" t="s">
+      <c r="A41" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B41" s="241">
+      <c r="B41" s="227">
         <v>363</v>
       </c>
     </row>
@@ -52259,39 +52575,39 @@
       <c r="A42" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="B42" s="241">
+      <c r="B42" s="227">
         <v>1256</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="240" t="s">
+      <c r="A43" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B43" s="241">
+      <c r="B43" s="227">
         <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="240" t="s">
+      <c r="A44" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B44" s="241">
+      <c r="B44" s="227">
         <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="240" t="s">
+      <c r="A45" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="241">
+      <c r="B45" s="227">
         <v>300</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="240" t="s">
+      <c r="A46" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B46" s="241">
+      <c r="B46" s="227">
         <v>370</v>
       </c>
     </row>
@@ -52299,39 +52615,39 @@
       <c r="A47" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="B47" s="241">
+      <c r="B47" s="227">
         <v>1311</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="240" t="s">
+      <c r="A48" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B48" s="241">
+      <c r="B48" s="227">
         <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="240" t="s">
+      <c r="A49" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="241">
+      <c r="B49" s="227">
         <v>288</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="240" t="s">
+      <c r="A50" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="241">
+      <c r="B50" s="227">
         <v>306</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="240" t="s">
+      <c r="A51" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B51" s="241">
+      <c r="B51" s="227">
         <v>386</v>
       </c>
     </row>
@@ -52339,39 +52655,39 @@
       <c r="A52" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="B52" s="241">
+      <c r="B52" s="227">
         <v>1333</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="240" t="s">
+      <c r="A53" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B53" s="241">
+      <c r="B53" s="227">
         <v>335</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="240" t="s">
+      <c r="A54" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B54" s="241">
+      <c r="B54" s="227">
         <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="240" t="s">
+      <c r="A55" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B55" s="241">
+      <c r="B55" s="227">
         <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="240" t="s">
+      <c r="A56" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B56" s="241">
+      <c r="B56" s="227">
         <v>402</v>
       </c>
     </row>
@@ -52379,39 +52695,39 @@
       <c r="A57" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="B57" s="241">
+      <c r="B57" s="227">
         <v>1399</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="240" t="s">
+      <c r="A58" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="241">
+      <c r="B58" s="227">
         <v>353</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="240" t="s">
+      <c r="A59" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="241">
+      <c r="B59" s="227">
         <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="240" t="s">
+      <c r="A60" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B60" s="241">
+      <c r="B60" s="227">
         <v>325</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="240" t="s">
+      <c r="A61" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B61" s="241">
+      <c r="B61" s="227">
         <v>405</v>
       </c>
     </row>
@@ -52419,39 +52735,39 @@
       <c r="A62" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B62" s="241">
+      <c r="B62" s="227">
         <v>1481</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="240" t="s">
+      <c r="A63" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B63" s="241">
+      <c r="B63" s="227">
         <v>393</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="240" t="s">
+      <c r="A64" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="241">
+      <c r="B64" s="227">
         <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="240" t="s">
+      <c r="A65" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B65" s="241">
+      <c r="B65" s="227">
         <v>327</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="240" t="s">
+      <c r="A66" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B66" s="241">
+      <c r="B66" s="227">
         <v>442</v>
       </c>
     </row>
@@ -52459,39 +52775,39 @@
       <c r="A67" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="B67" s="241">
+      <c r="B67" s="227">
         <v>1522</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="240" t="s">
+      <c r="A68" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B68" s="241">
+      <c r="B68" s="227">
         <v>383</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="240" t="s">
+      <c r="A69" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B69" s="241">
+      <c r="B69" s="227">
         <v>332</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="240" t="s">
+      <c r="A70" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B70" s="241">
+      <c r="B70" s="227">
         <v>361</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="240" t="s">
+      <c r="A71" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B71" s="241">
+      <c r="B71" s="227">
         <v>446</v>
       </c>
     </row>
@@ -52499,39 +52815,39 @@
       <c r="A72" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="B72" s="241">
+      <c r="B72" s="227">
         <v>1584</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="240" t="s">
+      <c r="A73" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B73" s="241">
+      <c r="B73" s="227">
         <v>387</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="240" t="s">
+      <c r="A74" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B74" s="241">
+      <c r="B74" s="227">
         <v>357</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="240" t="s">
+      <c r="A75" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B75" s="241">
+      <c r="B75" s="227">
         <v>374</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="240" t="s">
+      <c r="A76" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B76" s="241">
+      <c r="B76" s="227">
         <v>466</v>
       </c>
     </row>
@@ -52539,39 +52855,39 @@
       <c r="A77" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B77" s="241">
+      <c r="B77" s="227">
         <v>1646</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="240" t="s">
+      <c r="A78" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B78" s="241">
+      <c r="B78" s="227">
         <v>410</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="240" t="s">
+      <c r="A79" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B79" s="241">
+      <c r="B79" s="227">
         <v>370</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="240" t="s">
+      <c r="A80" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B80" s="241">
+      <c r="B80" s="227">
         <v>379</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="240" t="s">
+      <c r="A81" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B81" s="241">
+      <c r="B81" s="227">
         <v>487</v>
       </c>
     </row>
@@ -52579,39 +52895,39 @@
       <c r="A82" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="B82" s="241">
+      <c r="B82" s="227">
         <v>1695</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="240" t="s">
+      <c r="A83" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B83" s="241">
+      <c r="B83" s="227">
         <v>419</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="240" t="s">
+      <c r="A84" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B84" s="241">
+      <c r="B84" s="227">
         <v>377</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="240" t="s">
+      <c r="A85" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B85" s="241">
+      <c r="B85" s="227">
         <v>393</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="240" t="s">
+      <c r="A86" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B86" s="241">
+      <c r="B86" s="227">
         <v>506</v>
       </c>
     </row>
@@ -52619,39 +52935,39 @@
       <c r="A87" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B87" s="241">
+      <c r="B87" s="227">
         <v>1837</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="240" t="s">
+      <c r="A88" s="226" t="s">
         <v>110</v>
       </c>
-      <c r="B88" s="241">
+      <c r="B88" s="227">
         <v>458</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="240" t="s">
+      <c r="A89" s="226" t="s">
         <v>111</v>
       </c>
-      <c r="B89" s="241">
+      <c r="B89" s="227">
         <v>387</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="240" t="s">
+      <c r="A90" s="226" t="s">
         <v>112</v>
       </c>
-      <c r="B90" s="241">
+      <c r="B90" s="227">
         <v>427</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="240" t="s">
+      <c r="A91" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="B91" s="241">
+      <c r="B91" s="227">
         <v>565</v>
       </c>
     </row>
@@ -52659,7 +52975,7 @@
       <c r="A92" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="241">
+      <c r="B92" s="227">
         <v>23792</v>
       </c>
     </row>
@@ -54724,7 +55040,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54809,61 +55125,61 @@
       <c r="A3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="241">
+      <c r="B3" s="227">
         <v>284</v>
       </c>
-      <c r="C3" s="241">
+      <c r="C3" s="227">
         <v>262</v>
       </c>
-      <c r="D3" s="241">
+      <c r="D3" s="227">
         <v>272</v>
       </c>
-      <c r="E3" s="241">
+      <c r="E3" s="227">
         <v>261</v>
       </c>
-      <c r="F3" s="241">
+      <c r="F3" s="227">
         <v>286</v>
       </c>
-      <c r="G3" s="241">
+      <c r="G3" s="227">
         <v>295</v>
       </c>
-      <c r="H3" s="241">
+      <c r="H3" s="227">
         <v>279</v>
       </c>
-      <c r="I3" s="241">
+      <c r="I3" s="227">
         <v>294</v>
       </c>
-      <c r="J3" s="241">
+      <c r="J3" s="227">
         <v>313</v>
       </c>
-      <c r="K3" s="241">
+      <c r="K3" s="227">
         <v>331</v>
       </c>
-      <c r="L3" s="241">
+      <c r="L3" s="227">
         <v>335</v>
       </c>
-      <c r="M3" s="241">
+      <c r="M3" s="227">
         <v>353</v>
       </c>
-      <c r="N3" s="241">
+      <c r="N3" s="227">
         <v>393</v>
       </c>
-      <c r="O3" s="241">
+      <c r="O3" s="227">
         <v>383</v>
       </c>
-      <c r="P3" s="241">
+      <c r="P3" s="227">
         <v>387</v>
       </c>
-      <c r="Q3" s="241">
+      <c r="Q3" s="227">
         <v>410</v>
       </c>
-      <c r="R3" s="241">
+      <c r="R3" s="227">
         <v>419</v>
       </c>
-      <c r="S3" s="241">
+      <c r="S3" s="227">
         <v>458</v>
       </c>
-      <c r="T3" s="241">
+      <c r="T3" s="227">
         <v>6015</v>
       </c>
     </row>
@@ -54871,61 +55187,61 @@
       <c r="A4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="241">
+      <c r="B4" s="227">
         <v>213</v>
       </c>
-      <c r="C4" s="241">
+      <c r="C4" s="227">
         <v>228</v>
       </c>
-      <c r="D4" s="241">
+      <c r="D4" s="227">
         <v>233</v>
       </c>
-      <c r="E4" s="241">
+      <c r="E4" s="227">
         <v>227</v>
       </c>
-      <c r="F4" s="241">
+      <c r="F4" s="227">
         <v>227</v>
       </c>
-      <c r="G4" s="241">
+      <c r="G4" s="227">
         <v>233</v>
       </c>
-      <c r="H4" s="241">
+      <c r="H4" s="227">
         <v>250</v>
       </c>
-      <c r="I4" s="241">
+      <c r="I4" s="227">
         <v>255</v>
       </c>
-      <c r="J4" s="241">
+      <c r="J4" s="227">
         <v>273</v>
       </c>
-      <c r="K4" s="241">
+      <c r="K4" s="227">
         <v>288</v>
       </c>
-      <c r="L4" s="241">
+      <c r="L4" s="227">
         <v>288</v>
       </c>
-      <c r="M4" s="241">
+      <c r="M4" s="227">
         <v>316</v>
       </c>
-      <c r="N4" s="241">
+      <c r="N4" s="227">
         <v>319</v>
       </c>
-      <c r="O4" s="241">
+      <c r="O4" s="227">
         <v>332</v>
       </c>
-      <c r="P4" s="241">
+      <c r="P4" s="227">
         <v>357</v>
       </c>
-      <c r="Q4" s="241">
+      <c r="Q4" s="227">
         <v>370</v>
       </c>
-      <c r="R4" s="241">
+      <c r="R4" s="227">
         <v>377</v>
       </c>
-      <c r="S4" s="241">
+      <c r="S4" s="227">
         <v>387</v>
       </c>
-      <c r="T4" s="241">
+      <c r="T4" s="227">
         <v>5173</v>
       </c>
     </row>
@@ -54933,61 +55249,61 @@
       <c r="A5" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B5" s="241">
+      <c r="B5" s="227">
         <v>227</v>
       </c>
-      <c r="C5" s="241">
+      <c r="C5" s="227">
         <v>236</v>
       </c>
-      <c r="D5" s="241">
+      <c r="D5" s="227">
         <v>237</v>
       </c>
-      <c r="E5" s="241">
+      <c r="E5" s="227">
         <v>250</v>
       </c>
-      <c r="F5" s="241">
+      <c r="F5" s="227">
         <v>260</v>
       </c>
-      <c r="G5" s="241">
+      <c r="G5" s="227">
         <v>257</v>
       </c>
-      <c r="H5" s="241">
+      <c r="H5" s="227">
         <v>270</v>
       </c>
-      <c r="I5" s="241">
+      <c r="I5" s="227">
         <v>278</v>
       </c>
-      <c r="J5" s="241">
+      <c r="J5" s="227">
         <v>300</v>
       </c>
-      <c r="K5" s="241">
+      <c r="K5" s="227">
         <v>306</v>
       </c>
-      <c r="L5" s="241">
+      <c r="L5" s="227">
         <v>308</v>
       </c>
-      <c r="M5" s="241">
+      <c r="M5" s="227">
         <v>325</v>
       </c>
-      <c r="N5" s="241">
+      <c r="N5" s="227">
         <v>327</v>
       </c>
-      <c r="O5" s="241">
+      <c r="O5" s="227">
         <v>361</v>
       </c>
-      <c r="P5" s="241">
+      <c r="P5" s="227">
         <v>374</v>
       </c>
-      <c r="Q5" s="241">
+      <c r="Q5" s="227">
         <v>379</v>
       </c>
-      <c r="R5" s="241">
+      <c r="R5" s="227">
         <v>393</v>
       </c>
-      <c r="S5" s="241">
+      <c r="S5" s="227">
         <v>427</v>
       </c>
-      <c r="T5" s="241">
+      <c r="T5" s="227">
         <v>5515</v>
       </c>
     </row>
@@ -54995,61 +55311,61 @@
       <c r="A6" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B6" s="241">
+      <c r="B6" s="227">
         <v>308</v>
       </c>
-      <c r="C6" s="241">
+      <c r="C6" s="227">
         <v>320</v>
       </c>
-      <c r="D6" s="241">
+      <c r="D6" s="227">
         <v>313</v>
       </c>
-      <c r="E6" s="241">
+      <c r="E6" s="227">
         <v>314</v>
       </c>
-      <c r="F6" s="241">
+      <c r="F6" s="227">
         <v>311</v>
       </c>
-      <c r="G6" s="241">
+      <c r="G6" s="227">
         <v>339</v>
       </c>
-      <c r="H6" s="241">
+      <c r="H6" s="227">
         <v>346</v>
       </c>
-      <c r="I6" s="241">
+      <c r="I6" s="227">
         <v>363</v>
       </c>
-      <c r="J6" s="241">
+      <c r="J6" s="227">
         <v>370</v>
       </c>
-      <c r="K6" s="241">
+      <c r="K6" s="227">
         <v>386</v>
       </c>
-      <c r="L6" s="241">
+      <c r="L6" s="227">
         <v>402</v>
       </c>
-      <c r="M6" s="241">
+      <c r="M6" s="227">
         <v>405</v>
       </c>
-      <c r="N6" s="241">
+      <c r="N6" s="227">
         <v>442</v>
       </c>
-      <c r="O6" s="241">
+      <c r="O6" s="227">
         <v>446</v>
       </c>
-      <c r="P6" s="241">
+      <c r="P6" s="227">
         <v>466</v>
       </c>
-      <c r="Q6" s="241">
+      <c r="Q6" s="227">
         <v>487</v>
       </c>
-      <c r="R6" s="241">
+      <c r="R6" s="227">
         <v>506</v>
       </c>
-      <c r="S6" s="241">
+      <c r="S6" s="227">
         <v>565</v>
       </c>
-      <c r="T6" s="241">
+      <c r="T6" s="227">
         <v>7089</v>
       </c>
     </row>
@@ -55057,61 +55373,61 @@
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="241">
+      <c r="B7" s="227">
         <v>1032</v>
       </c>
-      <c r="C7" s="241">
+      <c r="C7" s="227">
         <v>1046</v>
       </c>
-      <c r="D7" s="241">
+      <c r="D7" s="227">
         <v>1055</v>
       </c>
-      <c r="E7" s="241">
+      <c r="E7" s="227">
         <v>1052</v>
       </c>
-      <c r="F7" s="241">
+      <c r="F7" s="227">
         <v>1084</v>
       </c>
-      <c r="G7" s="241">
+      <c r="G7" s="227">
         <v>1124</v>
       </c>
-      <c r="H7" s="241">
+      <c r="H7" s="227">
         <v>1145</v>
       </c>
-      <c r="I7" s="241">
+      <c r="I7" s="227">
         <v>1190</v>
       </c>
-      <c r="J7" s="241">
+      <c r="J7" s="227">
         <v>1256</v>
       </c>
-      <c r="K7" s="241">
+      <c r="K7" s="227">
         <v>1311</v>
       </c>
-      <c r="L7" s="241">
+      <c r="L7" s="227">
         <v>1333</v>
       </c>
-      <c r="M7" s="241">
+      <c r="M7" s="227">
         <v>1399</v>
       </c>
-      <c r="N7" s="241">
+      <c r="N7" s="227">
         <v>1481</v>
       </c>
-      <c r="O7" s="241">
+      <c r="O7" s="227">
         <v>1522</v>
       </c>
-      <c r="P7" s="241">
+      <c r="P7" s="227">
         <v>1584</v>
       </c>
-      <c r="Q7" s="241">
+      <c r="Q7" s="227">
         <v>1646</v>
       </c>
-      <c r="R7" s="241">
+      <c r="R7" s="227">
         <v>1695</v>
       </c>
-      <c r="S7" s="241">
+      <c r="S7" s="227">
         <v>1837</v>
       </c>
-      <c r="T7" s="241">
+      <c r="T7" s="227">
         <v>23792</v>
       </c>
     </row>
@@ -56072,19 +56388,19 @@
         <v>278</v>
       </c>
       <c r="D3" s="93"/>
-      <c r="H3" s="230" t="s">
+      <c r="H3" s="233" t="s">
         <v>277</v>
       </c>
-      <c r="I3" s="227"/>
+      <c r="I3" s="230"/>
     </row>
     <row r="4" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="95"/>
       <c r="C4" s="97"/>
       <c r="D4" s="93"/>
-      <c r="G4" s="230" t="s">
+      <c r="G4" s="233" t="s">
         <v>279</v>
       </c>
-      <c r="H4" s="227"/>
+      <c r="H4" s="230"/>
       <c r="I4" s="96"/>
     </row>
     <row r="5" spans="2:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -56093,17 +56409,17 @@
         <v>279</v>
       </c>
       <c r="D5" s="93"/>
-      <c r="G5" s="231"/>
-      <c r="H5" s="232"/>
+      <c r="G5" s="234"/>
+      <c r="H5" s="235"/>
     </row>
     <row r="6" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="95"/>
       <c r="C6" s="97"/>
       <c r="D6" s="93"/>
-      <c r="F6" s="226" t="s">
+      <c r="F6" s="229" t="s">
         <v>278</v>
       </c>
-      <c r="G6" s="227"/>
+      <c r="G6" s="230"/>
       <c r="H6" s="96"/>
     </row>
     <row r="7" spans="2:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -56112,8 +56428,8 @@
         <v>277</v>
       </c>
       <c r="D7" s="93"/>
-      <c r="F7" s="228"/>
-      <c r="G7" s="229"/>
+      <c r="F7" s="231"/>
+      <c r="G7" s="232"/>
     </row>
     <row r="8" spans="2:9" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="92"/>
@@ -56437,7 +56753,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56482,19 +56798,19 @@
       <c r="A3" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="B3" s="241">
+      <c r="B3" s="227">
         <v>284</v>
       </c>
-      <c r="C3" s="241">
+      <c r="C3" s="227">
         <v>213</v>
       </c>
-      <c r="D3" s="241">
+      <c r="D3" s="227">
         <v>227</v>
       </c>
-      <c r="E3" s="241">
+      <c r="E3" s="227">
         <v>308</v>
       </c>
-      <c r="F3" s="241">
+      <c r="F3" s="227">
         <v>1032</v>
       </c>
     </row>
@@ -56502,19 +56818,19 @@
       <c r="A4" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="241">
+      <c r="B4" s="227">
         <v>262</v>
       </c>
-      <c r="C4" s="241">
+      <c r="C4" s="227">
         <v>228</v>
       </c>
-      <c r="D4" s="241">
+      <c r="D4" s="227">
         <v>236</v>
       </c>
-      <c r="E4" s="241">
+      <c r="E4" s="227">
         <v>320</v>
       </c>
-      <c r="F4" s="241">
+      <c r="F4" s="227">
         <v>1046</v>
       </c>
     </row>
@@ -56522,19 +56838,19 @@
       <c r="A5" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="B5" s="241">
+      <c r="B5" s="227">
         <v>272</v>
       </c>
-      <c r="C5" s="241">
+      <c r="C5" s="227">
         <v>233</v>
       </c>
-      <c r="D5" s="241">
+      <c r="D5" s="227">
         <v>237</v>
       </c>
-      <c r="E5" s="241">
+      <c r="E5" s="227">
         <v>313</v>
       </c>
-      <c r="F5" s="241">
+      <c r="F5" s="227">
         <v>1055</v>
       </c>
     </row>
@@ -56542,19 +56858,19 @@
       <c r="A6" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="B6" s="241">
+      <c r="B6" s="227">
         <v>261</v>
       </c>
-      <c r="C6" s="241">
+      <c r="C6" s="227">
         <v>227</v>
       </c>
-      <c r="D6" s="241">
+      <c r="D6" s="227">
         <v>250</v>
       </c>
-      <c r="E6" s="241">
+      <c r="E6" s="227">
         <v>314</v>
       </c>
-      <c r="F6" s="241">
+      <c r="F6" s="227">
         <v>1052</v>
       </c>
     </row>
@@ -56562,19 +56878,19 @@
       <c r="A7" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="B7" s="241">
+      <c r="B7" s="227">
         <v>286</v>
       </c>
-      <c r="C7" s="241">
+      <c r="C7" s="227">
         <v>227</v>
       </c>
-      <c r="D7" s="241">
+      <c r="D7" s="227">
         <v>260</v>
       </c>
-      <c r="E7" s="241">
+      <c r="E7" s="227">
         <v>311</v>
       </c>
-      <c r="F7" s="241">
+      <c r="F7" s="227">
         <v>1084</v>
       </c>
     </row>
@@ -56582,19 +56898,19 @@
       <c r="A8" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="B8" s="241">
+      <c r="B8" s="227">
         <v>295</v>
       </c>
-      <c r="C8" s="241">
+      <c r="C8" s="227">
         <v>233</v>
       </c>
-      <c r="D8" s="241">
+      <c r="D8" s="227">
         <v>257</v>
       </c>
-      <c r="E8" s="241">
+      <c r="E8" s="227">
         <v>339</v>
       </c>
-      <c r="F8" s="241">
+      <c r="F8" s="227">
         <v>1124</v>
       </c>
     </row>
@@ -56602,19 +56918,19 @@
       <c r="A9" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="B9" s="241">
+      <c r="B9" s="227">
         <v>279</v>
       </c>
-      <c r="C9" s="241">
+      <c r="C9" s="227">
         <v>250</v>
       </c>
-      <c r="D9" s="241">
+      <c r="D9" s="227">
         <v>270</v>
       </c>
-      <c r="E9" s="241">
+      <c r="E9" s="227">
         <v>346</v>
       </c>
-      <c r="F9" s="241">
+      <c r="F9" s="227">
         <v>1145</v>
       </c>
     </row>
@@ -56622,19 +56938,19 @@
       <c r="A10" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="B10" s="241">
+      <c r="B10" s="227">
         <v>294</v>
       </c>
-      <c r="C10" s="241">
+      <c r="C10" s="227">
         <v>255</v>
       </c>
-      <c r="D10" s="241">
+      <c r="D10" s="227">
         <v>278</v>
       </c>
-      <c r="E10" s="241">
+      <c r="E10" s="227">
         <v>363</v>
       </c>
-      <c r="F10" s="241">
+      <c r="F10" s="227">
         <v>1190</v>
       </c>
     </row>
@@ -56642,19 +56958,19 @@
       <c r="A11" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="B11" s="241">
+      <c r="B11" s="227">
         <v>313</v>
       </c>
-      <c r="C11" s="241">
+      <c r="C11" s="227">
         <v>273</v>
       </c>
-      <c r="D11" s="241">
+      <c r="D11" s="227">
         <v>300</v>
       </c>
-      <c r="E11" s="241">
+      <c r="E11" s="227">
         <v>370</v>
       </c>
-      <c r="F11" s="241">
+      <c r="F11" s="227">
         <v>1256</v>
       </c>
     </row>
@@ -56662,19 +56978,19 @@
       <c r="A12" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="B12" s="241">
+      <c r="B12" s="227">
         <v>331</v>
       </c>
-      <c r="C12" s="241">
+      <c r="C12" s="227">
         <v>288</v>
       </c>
-      <c r="D12" s="241">
+      <c r="D12" s="227">
         <v>306</v>
       </c>
-      <c r="E12" s="241">
+      <c r="E12" s="227">
         <v>386</v>
       </c>
-      <c r="F12" s="241">
+      <c r="F12" s="227">
         <v>1311</v>
       </c>
     </row>
@@ -56682,19 +56998,19 @@
       <c r="A13" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="B13" s="241">
+      <c r="B13" s="227">
         <v>335</v>
       </c>
-      <c r="C13" s="241">
+      <c r="C13" s="227">
         <v>288</v>
       </c>
-      <c r="D13" s="241">
+      <c r="D13" s="227">
         <v>308</v>
       </c>
-      <c r="E13" s="241">
+      <c r="E13" s="227">
         <v>402</v>
       </c>
-      <c r="F13" s="241">
+      <c r="F13" s="227">
         <v>1333</v>
       </c>
     </row>
@@ -56702,19 +57018,19 @@
       <c r="A14" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="B14" s="241">
+      <c r="B14" s="227">
         <v>353</v>
       </c>
-      <c r="C14" s="241">
+      <c r="C14" s="227">
         <v>316</v>
       </c>
-      <c r="D14" s="241">
+      <c r="D14" s="227">
         <v>325</v>
       </c>
-      <c r="E14" s="241">
+      <c r="E14" s="227">
         <v>405</v>
       </c>
-      <c r="F14" s="241">
+      <c r="F14" s="227">
         <v>1399</v>
       </c>
     </row>
@@ -56722,19 +57038,19 @@
       <c r="A15" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="B15" s="241">
+      <c r="B15" s="227">
         <v>393</v>
       </c>
-      <c r="C15" s="241">
+      <c r="C15" s="227">
         <v>319</v>
       </c>
-      <c r="D15" s="241">
+      <c r="D15" s="227">
         <v>327</v>
       </c>
-      <c r="E15" s="241">
+      <c r="E15" s="227">
         <v>442</v>
       </c>
-      <c r="F15" s="241">
+      <c r="F15" s="227">
         <v>1481</v>
       </c>
     </row>
@@ -56742,19 +57058,19 @@
       <c r="A16" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="B16" s="241">
+      <c r="B16" s="227">
         <v>383</v>
       </c>
-      <c r="C16" s="241">
+      <c r="C16" s="227">
         <v>332</v>
       </c>
-      <c r="D16" s="241">
+      <c r="D16" s="227">
         <v>361</v>
       </c>
-      <c r="E16" s="241">
+      <c r="E16" s="227">
         <v>446</v>
       </c>
-      <c r="F16" s="241">
+      <c r="F16" s="227">
         <v>1522</v>
       </c>
     </row>
@@ -56762,19 +57078,19 @@
       <c r="A17" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="B17" s="241">
+      <c r="B17" s="227">
         <v>387</v>
       </c>
-      <c r="C17" s="241">
+      <c r="C17" s="227">
         <v>357</v>
       </c>
-      <c r="D17" s="241">
+      <c r="D17" s="227">
         <v>374</v>
       </c>
-      <c r="E17" s="241">
+      <c r="E17" s="227">
         <v>466</v>
       </c>
-      <c r="F17" s="241">
+      <c r="F17" s="227">
         <v>1584</v>
       </c>
     </row>
@@ -56782,19 +57098,19 @@
       <c r="A18" s="3" t="s">
         <v>444</v>
       </c>
-      <c r="B18" s="241">
+      <c r="B18" s="227">
         <v>410</v>
       </c>
-      <c r="C18" s="241">
+      <c r="C18" s="227">
         <v>370</v>
       </c>
-      <c r="D18" s="241">
+      <c r="D18" s="227">
         <v>379</v>
       </c>
-      <c r="E18" s="241">
+      <c r="E18" s="227">
         <v>487</v>
       </c>
-      <c r="F18" s="241">
+      <c r="F18" s="227">
         <v>1646</v>
       </c>
     </row>
@@ -56802,19 +57118,19 @@
       <c r="A19" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="B19" s="241">
+      <c r="B19" s="227">
         <v>419</v>
       </c>
-      <c r="C19" s="241">
+      <c r="C19" s="227">
         <v>377</v>
       </c>
-      <c r="D19" s="241">
+      <c r="D19" s="227">
         <v>393</v>
       </c>
-      <c r="E19" s="241">
+      <c r="E19" s="227">
         <v>506</v>
       </c>
-      <c r="F19" s="241">
+      <c r="F19" s="227">
         <v>1695</v>
       </c>
     </row>
@@ -56822,19 +57138,19 @@
       <c r="A20" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="B20" s="241">
+      <c r="B20" s="227">
         <v>458</v>
       </c>
-      <c r="C20" s="241">
+      <c r="C20" s="227">
         <v>387</v>
       </c>
-      <c r="D20" s="241">
+      <c r="D20" s="227">
         <v>427</v>
       </c>
-      <c r="E20" s="241">
+      <c r="E20" s="227">
         <v>565</v>
       </c>
-      <c r="F20" s="241">
+      <c r="F20" s="227">
         <v>1837</v>
       </c>
     </row>
@@ -56842,19 +57158,19 @@
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="241">
+      <c r="B21" s="227">
         <v>6015</v>
       </c>
-      <c r="C21" s="241">
+      <c r="C21" s="227">
         <v>5173</v>
       </c>
-      <c r="D21" s="241">
+      <c r="D21" s="227">
         <v>5515</v>
       </c>
-      <c r="E21" s="241">
+      <c r="E21" s="227">
         <v>7089</v>
       </c>
-      <c r="F21" s="241">
+      <c r="F21" s="227">
         <v>23792</v>
       </c>
     </row>
@@ -57601,10 +57917,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="233" t="s">
+      <c r="B2" s="236" t="s">
         <v>354</v>
       </c>
-      <c r="C2" s="233"/>
+      <c r="C2" s="236"/>
     </row>
     <row r="4" spans="2:3" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="202" t="s">
@@ -60416,7 +60732,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="234" t="s">
+      <c r="B14" s="237" t="s">
         <v>224</v>
       </c>
       <c r="C14" s="64" t="s">
@@ -60427,7 +60743,7 @@
       <c r="F14" s="64"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B15" s="235"/>
+      <c r="B15" s="238"/>
       <c r="C15" s="64" t="s">
         <v>219</v>
       </c>
@@ -60436,7 +60752,7 @@
       <c r="F15" s="64"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B16" s="236"/>
+      <c r="B16" s="239"/>
       <c r="C16" s="64" t="s">
         <v>220</v>
       </c>
@@ -61041,13 +61357,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="240" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="197" t="s">

</xml_diff>